<commit_message>
Commit: Create data - Student/Preferences data creation update to student number creation to avoid duplication
</commit_message>
<xml_diff>
--- a/Students&Preferences(60).xlsx
+++ b/Students&Preferences(60).xlsx
@@ -26,190 +26,190 @@
     <t>Preferences</t>
   </si>
   <si>
-    <t>Anthony Power</t>
+    <t>Keenan Clarke</t>
   </si>
   <si>
     <t>CS</t>
   </si>
   <si>
-    <t>Zak O'Leary</t>
-  </si>
-  <si>
-    <t>Cameron Lynch</t>
-  </si>
-  <si>
-    <t>John Cunningham</t>
-  </si>
-  <si>
-    <t>Reece Barry</t>
-  </si>
-  <si>
-    <t>Ruairi Fitzpatrick</t>
-  </si>
-  <si>
-    <t>Muhammad Brady</t>
-  </si>
-  <si>
-    <t>Kian Mullan</t>
-  </si>
-  <si>
-    <t>Jacques O'Farrell</t>
-  </si>
-  <si>
-    <t>Brian Foley</t>
-  </si>
-  <si>
-    <t>Kealan Flynn</t>
-  </si>
-  <si>
-    <t>Graeme O'Connor</t>
-  </si>
-  <si>
-    <t>Oran McGrath</t>
-  </si>
-  <si>
-    <t>Eric Regan</t>
-  </si>
-  <si>
-    <t>Donagh Duffy</t>
-  </si>
-  <si>
-    <t>Aaron Ryan</t>
-  </si>
-  <si>
-    <t>Gavin Martin</t>
-  </si>
-  <si>
-    <t>Rian Power</t>
-  </si>
-  <si>
-    <t>Marc O'Dwyer</t>
-  </si>
-  <si>
-    <t>Ryan Sweeney</t>
-  </si>
-  <si>
-    <t>Cody Bell</t>
-  </si>
-  <si>
-    <t>Cameron Flynn</t>
-  </si>
-  <si>
-    <t>Reuben Griffin</t>
-  </si>
-  <si>
-    <t>Craig O'Brien</t>
-  </si>
-  <si>
-    <t>Aron O'Doherty</t>
-  </si>
-  <si>
-    <t>Darrell Quinn</t>
-  </si>
-  <si>
-    <t>Owen O'Connor</t>
-  </si>
-  <si>
-    <t>Raymond Collins</t>
+    <t>Conrad O'Farrell</t>
+  </si>
+  <si>
+    <t>Raymond O'Callaghan</t>
+  </si>
+  <si>
+    <t>Larry McGrath</t>
+  </si>
+  <si>
+    <t>Dillon O'Callaghan</t>
+  </si>
+  <si>
+    <t>Benedict O'Connor</t>
+  </si>
+  <si>
+    <t>Gavan Sheehan</t>
+  </si>
+  <si>
+    <t>Deane Reid</t>
+  </si>
+  <si>
+    <t>Eoin O'Rourke</t>
+  </si>
+  <si>
+    <t>Albert O'Sullivan</t>
+  </si>
+  <si>
+    <t>Eimhin Kennedy</t>
+  </si>
+  <si>
+    <t>George O'Reilly</t>
+  </si>
+  <si>
+    <t>Kyran White</t>
   </si>
   <si>
     <t>Johnny Quinn</t>
   </si>
   <si>
-    <t>George MacDonald</t>
-  </si>
-  <si>
-    <t>Daire MacDonald</t>
-  </si>
-  <si>
-    <t>Henry Griffin</t>
-  </si>
-  <si>
-    <t>Khalid McLoughlin</t>
-  </si>
-  <si>
-    <t>Aidan Ryan</t>
-  </si>
-  <si>
-    <t>Charles O'Neill</t>
-  </si>
-  <si>
-    <t>Maximillian Wilson</t>
-  </si>
-  <si>
-    <t>Deaglan O'Connell</t>
+    <t>Tiernan Reid</t>
+  </si>
+  <si>
+    <t>Rowan Donovan</t>
+  </si>
+  <si>
+    <t>William Kenny</t>
+  </si>
+  <si>
+    <t>Oran Stewart</t>
+  </si>
+  <si>
+    <t>Andre Kennedy</t>
+  </si>
+  <si>
+    <t>Feargal Griffin</t>
+  </si>
+  <si>
+    <t>Marc O'Donnell</t>
+  </si>
+  <si>
+    <t>Tyrone Nolan</t>
+  </si>
+  <si>
+    <t>Aran O'Callaghan</t>
+  </si>
+  <si>
+    <t>Brain White</t>
+  </si>
+  <si>
+    <t>Casey Lynch</t>
+  </si>
+  <si>
+    <t>Tyler Brown</t>
+  </si>
+  <si>
+    <t>Jason Walsh</t>
+  </si>
+  <si>
+    <t>Ultan O'Callaghan</t>
+  </si>
+  <si>
+    <t>Conan Regan</t>
+  </si>
+  <si>
+    <t>Hugo Fitzgerald</t>
+  </si>
+  <si>
+    <t>Eamonn MacNamara</t>
+  </si>
+  <si>
+    <t>Leo Byrne</t>
+  </si>
+  <si>
+    <t>Zack O'Leary</t>
+  </si>
+  <si>
+    <t>Kieran Stewart</t>
+  </si>
+  <si>
+    <t>Jonathon Sweeney</t>
+  </si>
+  <si>
+    <t>Padhraic Smith</t>
+  </si>
+  <si>
+    <t>Caleb O'Keeffe</t>
   </si>
   <si>
     <t>DS</t>
   </si>
   <si>
-    <t>Hugh Campbell</t>
-  </si>
-  <si>
-    <t>Zach Murray</t>
-  </si>
-  <si>
-    <t>Dean King</t>
-  </si>
-  <si>
-    <t>Casey Stewart</t>
-  </si>
-  <si>
-    <t>Graeme Ryan</t>
-  </si>
-  <si>
-    <t>Anthony Healy</t>
-  </si>
-  <si>
-    <t>James Kenny</t>
-  </si>
-  <si>
-    <t>Kenneth Ryan</t>
-  </si>
-  <si>
-    <t>Dane Kavanagh</t>
-  </si>
-  <si>
-    <t>Garry Mullan</t>
-  </si>
-  <si>
-    <t>Tomas Power</t>
-  </si>
-  <si>
-    <t>Jesse MacNamara</t>
-  </si>
-  <si>
-    <t>Jay Stewart</t>
-  </si>
-  <si>
-    <t>Dominic Wilson</t>
-  </si>
-  <si>
-    <t>Mathew Cullen</t>
-  </si>
-  <si>
-    <t>Troy O'Neill</t>
-  </si>
-  <si>
-    <t>Aron Burke</t>
-  </si>
-  <si>
-    <t>Charlie Thompson</t>
-  </si>
-  <si>
-    <t>Johnathan Murray</t>
-  </si>
-  <si>
-    <t>Karl Hayes</t>
-  </si>
-  <si>
-    <t>Finbarr Collins</t>
-  </si>
-  <si>
-    <t>Niall Moore</t>
-  </si>
-  <si>
-    <t>Seamus Cullen</t>
+    <t>Euan O'Leary</t>
+  </si>
+  <si>
+    <t>George Burns</t>
+  </si>
+  <si>
+    <t>Noel Brady</t>
+  </si>
+  <si>
+    <t>Kelan Burns</t>
+  </si>
+  <si>
+    <t>Johnathan Byrne</t>
+  </si>
+  <si>
+    <t>Emmanuel Maguire</t>
+  </si>
+  <si>
+    <t>Kelvin Kane</t>
+  </si>
+  <si>
+    <t>Clive Murray</t>
+  </si>
+  <si>
+    <t>Damien Murray</t>
+  </si>
+  <si>
+    <t>Eamon Moore</t>
+  </si>
+  <si>
+    <t>Clayton Daly</t>
+  </si>
+  <si>
+    <t>Feargal MacDermott</t>
+  </si>
+  <si>
+    <t>Evan O'Callaghan</t>
+  </si>
+  <si>
+    <t>Rory Maher</t>
+  </si>
+  <si>
+    <t>Harry Foley</t>
+  </si>
+  <si>
+    <t>Darren O'Sullivan</t>
+  </si>
+  <si>
+    <t>Bernard Hayes</t>
+  </si>
+  <si>
+    <t>Louis White</t>
+  </si>
+  <si>
+    <t>Greg Flanagan</t>
+  </si>
+  <si>
+    <t>Finnan Reid</t>
+  </si>
+  <si>
+    <t>Samuel Thompson</t>
+  </si>
+  <si>
+    <t>Darragh Stewart</t>
+  </si>
+  <si>
+    <t>Mairtin Nolan</t>
   </si>
 </sst>
 </file>
@@ -266,7 +266,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="18.32421875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="20.640625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="16.2578125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.89453125" customWidth="true" bestFit="true"/>
@@ -291,7 +291,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>769729.0</v>
+        <v>943163.0</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -302,7 +302,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>116396.0</v>
+        <v>215954.0</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -313,7 +313,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>371242.0</v>
+        <v>483586.0</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -324,7 +324,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>337655.0</v>
+        <v>162616.0</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -335,7 +335,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>169713.0</v>
+        <v>413535.0</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -346,7 +346,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>249438.0</v>
+        <v>216821.0</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -357,7 +357,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>491733.0</v>
+        <v>242317.0</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -368,7 +368,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>427219.0</v>
+        <v>782668.0</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -379,7 +379,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>313657.0</v>
+        <v>639215.0</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -390,7 +390,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>678827.0</v>
+        <v>711912.0</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -401,7 +401,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>348255.0</v>
+        <v>897165.0</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -412,7 +412,7 @@
         <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>926392.0</v>
+        <v>967415.0</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -423,7 +423,7 @@
         <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>144877.0</v>
+        <v>864957.0</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -434,7 +434,7 @@
         <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>769248.0</v>
+        <v>318243.0</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -445,7 +445,7 @@
         <v>19</v>
       </c>
       <c r="B16" t="n">
-        <v>732569.0</v>
+        <v>334652.0</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -456,7 +456,7 @@
         <v>20</v>
       </c>
       <c r="B17" t="n">
-        <v>523628.0</v>
+        <v>411926.0</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -467,7 +467,7 @@
         <v>21</v>
       </c>
       <c r="B18" t="n">
-        <v>736359.0</v>
+        <v>164239.0</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -478,7 +478,7 @@
         <v>22</v>
       </c>
       <c r="B19" t="n">
-        <v>615325.0</v>
+        <v>985242.0</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -489,7 +489,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="n">
-        <v>525891.0</v>
+        <v>332325.0</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -500,7 +500,7 @@
         <v>24</v>
       </c>
       <c r="B21" t="n">
-        <v>116291.0</v>
+        <v>618255.0</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -511,7 +511,7 @@
         <v>25</v>
       </c>
       <c r="B22" t="n">
-        <v>198719.0</v>
+        <v>846263.0</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -522,7 +522,7 @@
         <v>26</v>
       </c>
       <c r="B23" t="n">
-        <v>538311.0</v>
+        <v>217494.0</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -533,7 +533,7 @@
         <v>27</v>
       </c>
       <c r="B24" t="n">
-        <v>854989.0</v>
+        <v>275951.0</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -544,7 +544,7 @@
         <v>28</v>
       </c>
       <c r="B25" t="n">
-        <v>393244.0</v>
+        <v>394631.0</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -555,7 +555,7 @@
         <v>29</v>
       </c>
       <c r="B26" t="n">
-        <v>968918.0</v>
+        <v>218418.0</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -566,7 +566,7 @@
         <v>30</v>
       </c>
       <c r="B27" t="n">
-        <v>323915.0</v>
+        <v>494149.0</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -577,7 +577,7 @@
         <v>31</v>
       </c>
       <c r="B28" t="n">
-        <v>466394.0</v>
+        <v>385338.0</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -588,7 +588,7 @@
         <v>32</v>
       </c>
       <c r="B29" t="n">
-        <v>817555.0</v>
+        <v>182343.0</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -599,7 +599,7 @@
         <v>33</v>
       </c>
       <c r="B30" t="n">
-        <v>916262.0</v>
+        <v>323432.0</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
@@ -610,7 +610,7 @@
         <v>34</v>
       </c>
       <c r="B31" t="n">
-        <v>318627.0</v>
+        <v>157144.0</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
@@ -621,7 +621,7 @@
         <v>35</v>
       </c>
       <c r="B32" t="n">
-        <v>318626.0</v>
+        <v>841774.0</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -632,7 +632,7 @@
         <v>36</v>
       </c>
       <c r="B33" t="n">
-        <v>425173.0</v>
+        <v>582614.0</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -643,7 +643,7 @@
         <v>37</v>
       </c>
       <c r="B34" t="n">
-        <v>684936.0</v>
+        <v>112379.0</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -654,7 +654,7 @@
         <v>38</v>
       </c>
       <c r="B35" t="n">
-        <v>245216.0</v>
+        <v>446258.0</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
@@ -665,7 +665,7 @@
         <v>39</v>
       </c>
       <c r="B36" t="n">
-        <v>223786.0</v>
+        <v>494649.0</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -676,7 +676,7 @@
         <v>40</v>
       </c>
       <c r="B37" t="n">
-        <v>128296.0</v>
+        <v>153199.0</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -687,7 +687,7 @@
         <v>41</v>
       </c>
       <c r="B38" t="n">
-        <v>865694.0</v>
+        <v>431754.0</v>
       </c>
       <c r="C38" t="s">
         <v>42</v>
@@ -698,7 +698,7 @@
         <v>43</v>
       </c>
       <c r="B39" t="n">
-        <v>182388.0</v>
+        <v>435261.0</v>
       </c>
       <c r="C39" t="s">
         <v>42</v>
@@ -709,7 +709,7 @@
         <v>44</v>
       </c>
       <c r="B40" t="n">
-        <v>895845.0</v>
+        <v>433533.0</v>
       </c>
       <c r="C40" t="s">
         <v>42</v>
@@ -720,7 +720,7 @@
         <v>45</v>
       </c>
       <c r="B41" t="n">
-        <v>273753.0</v>
+        <v>242413.0</v>
       </c>
       <c r="C41" t="s">
         <v>42</v>
@@ -731,7 +731,7 @@
         <v>46</v>
       </c>
       <c r="B42" t="n">
-        <v>192878.0</v>
+        <v>314467.0</v>
       </c>
       <c r="C42" t="s">
         <v>42</v>
@@ -742,7 +742,7 @@
         <v>47</v>
       </c>
       <c r="B43" t="n">
-        <v>267792.0</v>
+        <v>278833.0</v>
       </c>
       <c r="C43" t="s">
         <v>42</v>
@@ -753,7 +753,7 @@
         <v>48</v>
       </c>
       <c r="B44" t="n">
-        <v>495729.0</v>
+        <v>518575.0</v>
       </c>
       <c r="C44" t="s">
         <v>42</v>
@@ -764,7 +764,7 @@
         <v>49</v>
       </c>
       <c r="B45" t="n">
-        <v>818122.0</v>
+        <v>335635.0</v>
       </c>
       <c r="C45" t="s">
         <v>42</v>
@@ -775,7 +775,7 @@
         <v>50</v>
       </c>
       <c r="B46" t="n">
-        <v>912714.0</v>
+        <v>892753.0</v>
       </c>
       <c r="C46" t="s">
         <v>42</v>
@@ -786,7 +786,7 @@
         <v>51</v>
       </c>
       <c r="B47" t="n">
-        <v>183485.0</v>
+        <v>547634.0</v>
       </c>
       <c r="C47" t="s">
         <v>42</v>
@@ -797,7 +797,7 @@
         <v>52</v>
       </c>
       <c r="B48" t="n">
-        <v>377141.0</v>
+        <v>911749.0</v>
       </c>
       <c r="C48" t="s">
         <v>42</v>
@@ -808,7 +808,7 @@
         <v>53</v>
       </c>
       <c r="B49" t="n">
-        <v>538317.0</v>
+        <v>217149.0</v>
       </c>
       <c r="C49" t="s">
         <v>42</v>
@@ -819,7 +819,7 @@
         <v>54</v>
       </c>
       <c r="B50" t="n">
-        <v>256322.0</v>
+        <v>139559.0</v>
       </c>
       <c r="C50" t="s">
         <v>42</v>
@@ -830,7 +830,7 @@
         <v>55</v>
       </c>
       <c r="B51" t="n">
-        <v>937419.0</v>
+        <v>729126.0</v>
       </c>
       <c r="C51" t="s">
         <v>42</v>
@@ -841,7 +841,7 @@
         <v>56</v>
       </c>
       <c r="B52" t="n">
-        <v>385663.0</v>
+        <v>339635.0</v>
       </c>
       <c r="C52" t="s">
         <v>42</v>
@@ -852,7 +852,7 @@
         <v>57</v>
       </c>
       <c r="B53" t="n">
-        <v>141764.0</v>
+        <v>738232.0</v>
       </c>
       <c r="C53" t="s">
         <v>42</v>
@@ -863,7 +863,7 @@
         <v>58</v>
       </c>
       <c r="B54" t="n">
-        <v>589139.0</v>
+        <v>845522.0</v>
       </c>
       <c r="C54" t="s">
         <v>42</v>
@@ -874,7 +874,7 @@
         <v>59</v>
       </c>
       <c r="B55" t="n">
-        <v>552298.0</v>
+        <v>233691.0</v>
       </c>
       <c r="C55" t="s">
         <v>42</v>
@@ -885,7 +885,7 @@
         <v>60</v>
       </c>
       <c r="B56" t="n">
-        <v>911216.0</v>
+        <v>585966.0</v>
       </c>
       <c r="C56" t="s">
         <v>42</v>
@@ -896,7 +896,7 @@
         <v>61</v>
       </c>
       <c r="B57" t="n">
-        <v>246149.0</v>
+        <v>419246.0</v>
       </c>
       <c r="C57" t="s">
         <v>42</v>
@@ -907,7 +907,7 @@
         <v>62</v>
       </c>
       <c r="B58" t="n">
-        <v>624592.0</v>
+        <v>142247.0</v>
       </c>
       <c r="C58" t="s">
         <v>42</v>
@@ -918,7 +918,7 @@
         <v>63</v>
       </c>
       <c r="B59" t="n">
-        <v>327215.0</v>
+        <v>277775.0</v>
       </c>
       <c r="C59" t="s">
         <v>42</v>
@@ -929,7 +929,7 @@
         <v>64</v>
       </c>
       <c r="B60" t="n">
-        <v>348153.0</v>
+        <v>134182.0</v>
       </c>
       <c r="C60" t="s">
         <v>42</v>
@@ -940,7 +940,7 @@
         <v>65</v>
       </c>
       <c r="B61" t="n">
-        <v>965225.0</v>
+        <v>795535.0</v>
       </c>
       <c r="C61" t="s">
         <v>42</v>

</xml_diff>